<commit_message>
adapt example schedule to latest version
</commit_message>
<xml_diff>
--- a/scenarios/01_original_data/cargo_train_schedule.xlsx
+++ b/scenarios/01_original_data/cargo_train_schedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\eclipse-workspace\ibg\scenarios\01_original_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\eclipse-workspace\matsim-switzerland-freight\scenarios\01_original_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C4377F-00BA-478B-A632-833A1D8278A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1A5CC4-4B3E-43B3-8AE6-7DC664B96AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="936" windowWidth="21600" windowHeight="12672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21255" yWindow="3195" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$K$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$L$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
-  <si>
-    <t>Zug</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Richtung</t>
   </si>
@@ -101,6 +98,12 @@
   </si>
   <si>
     <t>DT-SC</t>
+  </si>
+  <si>
+    <t>Linie</t>
+  </si>
+  <si>
+    <t>Zugeinheiten</t>
   </si>
 </sst>
 </file>
@@ -328,33 +331,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -375,7 +373,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -673,272 +671,261 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E5" sqref="E5"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="27"/>
-    <col min="5" max="5" width="8.7109375" style="28"/>
-    <col min="6" max="6" width="7.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="27"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="27" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="22"/>
+    <col min="6" max="6" width="8.7109375" style="23"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="22"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="31" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="24"/>
-    </row>
-    <row r="2" spans="1:14" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33" t="s">
+      <c r="F2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="H2" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>6</v>
+      <c r="K2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="A3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="19">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="19">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
         <v>0.375</v>
       </c>
-      <c r="E3" s="16">
+      <c r="F3" s="16">
         <v>0.52083333333333337</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G3" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G3" s="10">
-        <f>E3+F3</f>
+      <c r="H3" s="10">
+        <f>F3+G3</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="13">
         <v>0.57291666666666663</v>
       </c>
-      <c r="I3" s="11">
+      <c r="J3" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J3" s="9">
-        <f>H3+I3</f>
+      <c r="K3" s="9">
+        <f>I3+J3</f>
         <v>0.59375</v>
       </c>
-      <c r="K3" s="26">
+      <c r="L3" s="21">
         <v>0.64583333333333337</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="19"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="22">
+      <c r="A4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="19">
         <v>2</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="19">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E4" s="15">
-        <f>G4+F4</f>
+      <c r="F4" s="15">
+        <f>H4+G4</f>
         <v>0.48958333333333331</v>
       </c>
-      <c r="F4" s="11">
+      <c r="G4" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G4" s="14">
+      <c r="H4" s="14">
         <v>0.46875</v>
       </c>
-      <c r="H4" s="9">
-        <f>J4+I4</f>
+      <c r="I4" s="9">
+        <f>K4+J4</f>
         <v>0.4375</v>
       </c>
-      <c r="I4" s="11">
+      <c r="J4" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="J4" s="13">
+      <c r="K4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K4" s="12">
+      <c r="L4" s="12">
         <v>0.36458333333333331</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="19"/>
+      <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="22">
+      <c r="A6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="19">
         <v>1</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="14">
+      <c r="D6" s="19">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="14">
         <v>0.5</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="12">
+      <c r="L6" s="21"/>
+      <c r="N6" s="12">
         <v>0.375</v>
       </c>
-      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="22">
+      <c r="A7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="19">
         <v>2</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9">
+      <c r="D7" s="19">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9">
         <v>0.625</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="26">
+      <c r="L7" s="7"/>
+      <c r="N7" s="21">
         <v>0.75</v>
       </c>
-      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="25"/>
-      <c r="N9" s="25"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="1048544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1048544" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K7" xr:uid="{A2F39999-98DD-4F29-9CE9-B5711A0A92DD}"/>
+  <autoFilter ref="A2:L7" xr:uid="{A2F39999-98DD-4F29-9CE9-B5711A0A92DD}"/>
   <mergeCells count="2">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>